<commit_message>
Mudanças na planilha de risco
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Risco.xlsx
+++ b/Documentação/Planilha de Risco.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela" sheetId="1" r:id="rId1"/>
@@ -256,9 +256,6 @@
     <t xml:space="preserve">O gestor de comunicações deverá ficar responsável por Identificar a fonte do problema em questão e se atentar à menções nas mídias referentes à empresa durante e pós crise. Para que com o tempo as coisas voltem ao normal </t>
   </si>
   <si>
-    <t xml:space="preserve">Em casos como esse custos devem ser cortados e planejamento </t>
-  </si>
-  <si>
     <t>Atraso na entrega do projeto</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
       </rPr>
       <t>-ALTA</t>
     </r>
+  </si>
+  <si>
+    <t>Em casos como esse, custos devem ser cortados e um planejamento emergencial deverá ser colocado em prática. Amenizar  o impacto financeiro através de organização e gerenciamento financeiro.</t>
   </si>
 </sst>
 </file>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +982,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>2</v>
@@ -1002,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
@@ -1075,7 +1075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18">
         <v>4</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18">
         <v>6</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>13</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>